<commit_message>
Refactor metrics calculations and improve data handling
- Updated `calculate_atl_ctl_tsb` to ensure total TSS is treated as float and used `adjust=False` for EWMA calculations.
- Enhanced `compute_all_metrics` to check for existence of TSS columns before filling NaN values, ensuring they are converted to float.
- Reindexed aggregated data to daily for accurate EWMA and rolling calculations.
- Improved handling of rolling metrics and added checks for column existence.
- Updated CSV output to reflect new metrics and ensure consistency in naming conventions.
- Adjusted plotting functions to check for the presence of TSB (EWMA) in the DataFrame before plotting.
- Modified utility functions to correctly reference updated column names for CTL and ATL metrics.
</commit_message>
<xml_diff>
--- a/data/master_log.xlsx
+++ b/data/master_log.xlsx
@@ -18,7 +18,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -57,11 +60,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -427,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AL1"/>
+  <dimension ref="A1:AL13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -625,6 +629,1398 @@
         <is>
           <t>Calories Burned</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="n">
+        <v>45976</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Build</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Cycling</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Indoor</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>3</v>
+      </c>
+      <c r="F2" t="n">
+        <v>54</v>
+      </c>
+      <c r="G2" t="n">
+        <v>18</v>
+      </c>
+      <c r="H2" t="n">
+        <v>84</v>
+      </c>
+      <c r="I2" t="n">
+        <v>265</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Zone 3</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Mix</t>
+        </is>
+      </c>
+      <c r="L2" t="n">
+        <v>8</v>
+      </c>
+      <c r="M2" t="n">
+        <v>87</v>
+      </c>
+      <c r="N2" t="n">
+        <v>89</v>
+      </c>
+      <c r="O2" t="n">
+        <v>358</v>
+      </c>
+      <c r="P2" t="n">
+        <v>60</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>2240</v>
+      </c>
+      <c r="R2" t="n">
+        <v>746.6666666666666</v>
+      </c>
+      <c r="S2" t="n">
+        <v>156</v>
+      </c>
+      <c r="T2" t="n">
+        <v>123</v>
+      </c>
+      <c r="U2" t="n">
+        <v>10</v>
+      </c>
+      <c r="V2" t="n">
+        <v>120</v>
+      </c>
+      <c r="W2" t="n">
+        <v>50</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z2" t="inlineStr"/>
+      <c r="AA2" t="inlineStr"/>
+      <c r="AB2" t="inlineStr"/>
+      <c r="AC2" t="inlineStr"/>
+      <c r="AD2" t="n">
+        <v>164.3792328579008</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>0.7402234636871509</v>
+      </c>
+      <c r="AG2" t="inlineStr"/>
+      <c r="AH2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>54</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>164.3792328579008</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>2862</v>
+      </c>
+      <c r="AL2" t="n">
+        <v>2718.9</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="n">
+        <v>45977</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Build</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Cycling</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Indoor</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" t="n">
+        <v>32</v>
+      </c>
+      <c r="G3" t="n">
+        <v>16.7</v>
+      </c>
+      <c r="H3" t="n">
+        <v>44</v>
+      </c>
+      <c r="I3" t="n">
+        <v>235</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Recovery</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Mix</t>
+        </is>
+      </c>
+      <c r="L3" t="n">
+        <v>6</v>
+      </c>
+      <c r="M3" t="n">
+        <v>77</v>
+      </c>
+      <c r="N3" t="n">
+        <v>54</v>
+      </c>
+      <c r="O3" t="n">
+        <v>358</v>
+      </c>
+      <c r="P3" t="n">
+        <v>60</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>2240</v>
+      </c>
+      <c r="R3" t="n">
+        <v>1120</v>
+      </c>
+      <c r="S3" t="n">
+        <v>137</v>
+      </c>
+      <c r="T3" t="n">
+        <v>117</v>
+      </c>
+      <c r="U3" t="n">
+        <v>60</v>
+      </c>
+      <c r="V3" t="n">
+        <v>60</v>
+      </c>
+      <c r="W3" t="n">
+        <v>0</v>
+      </c>
+      <c r="X3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z3" t="inlineStr"/>
+      <c r="AA3" t="inlineStr"/>
+      <c r="AB3" t="inlineStr"/>
+      <c r="AC3" t="inlineStr"/>
+      <c r="AD3" t="n">
+        <v>86.17864610967196</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>0.6564245810055865</v>
+      </c>
+      <c r="AG3" t="inlineStr"/>
+      <c r="AH3" t="n">
+        <v>2</v>
+      </c>
+      <c r="AI3" t="n">
+        <v>32</v>
+      </c>
+      <c r="AJ3" t="n">
+        <v>86.17864610967196</v>
+      </c>
+      <c r="AK3" t="n">
+        <v>1692</v>
+      </c>
+      <c r="AL3" t="n">
+        <v>1607.4</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="n">
+        <v>45978</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Build</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Cycling</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Indoor</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>2</v>
+      </c>
+      <c r="F4" t="n">
+        <v>45</v>
+      </c>
+      <c r="G4" t="n">
+        <v>18.9</v>
+      </c>
+      <c r="H4" t="n">
+        <v>67</v>
+      </c>
+      <c r="I4" t="n">
+        <v>280</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Zone 3</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Mix</t>
+        </is>
+      </c>
+      <c r="L4" t="n">
+        <v>7</v>
+      </c>
+      <c r="M4" t="n">
+        <v>87</v>
+      </c>
+      <c r="N4" t="n">
+        <v>67</v>
+      </c>
+      <c r="O4" t="n">
+        <v>358</v>
+      </c>
+      <c r="P4" t="n">
+        <v>60</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>2240</v>
+      </c>
+      <c r="R4" t="n">
+        <v>1120</v>
+      </c>
+      <c r="S4" t="n">
+        <v>155</v>
+      </c>
+      <c r="T4" t="n">
+        <v>129</v>
+      </c>
+      <c r="U4" t="n">
+        <v>5</v>
+      </c>
+      <c r="V4" t="n">
+        <v>115</v>
+      </c>
+      <c r="W4" t="n">
+        <v>0</v>
+      </c>
+      <c r="X4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z4" t="inlineStr"/>
+      <c r="AA4" t="inlineStr"/>
+      <c r="AB4" t="inlineStr"/>
+      <c r="AC4" t="inlineStr"/>
+      <c r="AD4" t="n">
+        <v>122.3432477138666</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>0.7821229050279329</v>
+      </c>
+      <c r="AG4" t="inlineStr"/>
+      <c r="AH4" t="n">
+        <v>2</v>
+      </c>
+      <c r="AI4" t="n">
+        <v>45</v>
+      </c>
+      <c r="AJ4" t="n">
+        <v>122.3432477138666</v>
+      </c>
+      <c r="AK4" t="n">
+        <v>2016</v>
+      </c>
+      <c r="AL4" t="n">
+        <v>1915.2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="n">
+        <v>45979</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Build</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Cycling</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Indoor</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>3</v>
+      </c>
+      <c r="F5" t="n">
+        <v>59</v>
+      </c>
+      <c r="G5" t="n">
+        <v>16.7</v>
+      </c>
+      <c r="H5" t="n">
+        <v>43</v>
+      </c>
+      <c r="I5" t="n">
+        <v>276</v>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Zone 3</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Mix</t>
+        </is>
+      </c>
+      <c r="L5" t="n">
+        <v>6</v>
+      </c>
+      <c r="M5" t="n">
+        <v>76</v>
+      </c>
+      <c r="N5" t="n">
+        <v>88</v>
+      </c>
+      <c r="O5" t="n">
+        <v>358</v>
+      </c>
+      <c r="P5" t="n">
+        <v>60</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>2240</v>
+      </c>
+      <c r="R5" t="n">
+        <v>746.6666666666666</v>
+      </c>
+      <c r="S5" t="n">
+        <v>154</v>
+      </c>
+      <c r="T5" t="n">
+        <v>123</v>
+      </c>
+      <c r="U5" t="n">
+        <v>20</v>
+      </c>
+      <c r="V5" t="n">
+        <v>120</v>
+      </c>
+      <c r="W5" t="n">
+        <v>40</v>
+      </c>
+      <c r="X5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z5" t="inlineStr"/>
+      <c r="AA5" t="inlineStr"/>
+      <c r="AB5" t="inlineStr"/>
+      <c r="AC5" t="inlineStr"/>
+      <c r="AD5" t="n">
+        <v>178.3090415405262</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>0.770949720670391</v>
+      </c>
+      <c r="AG5" t="inlineStr"/>
+      <c r="AH5" t="n">
+        <v>3</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>59</v>
+      </c>
+      <c r="AJ5" t="n">
+        <v>178.3090415405262</v>
+      </c>
+      <c r="AK5" t="n">
+        <v>2980.8</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>2831.76</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="n">
+        <v>45980</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Build</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Cycling</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Indoor</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>2</v>
+      </c>
+      <c r="F6" t="n">
+        <v>32</v>
+      </c>
+      <c r="G6" t="n">
+        <v>17.6</v>
+      </c>
+      <c r="H6" t="n">
+        <v>34</v>
+      </c>
+      <c r="I6" t="n">
+        <v>306</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Tempo</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Mix</t>
+        </is>
+      </c>
+      <c r="L6" t="n">
+        <v>9</v>
+      </c>
+      <c r="M6" t="n">
+        <v>89</v>
+      </c>
+      <c r="N6" t="n">
+        <v>59</v>
+      </c>
+      <c r="O6" t="n">
+        <v>358</v>
+      </c>
+      <c r="P6" t="n">
+        <v>60</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>2240</v>
+      </c>
+      <c r="R6" t="n">
+        <v>1120</v>
+      </c>
+      <c r="S6" t="n">
+        <v>167</v>
+      </c>
+      <c r="T6" t="n">
+        <v>132</v>
+      </c>
+      <c r="U6" t="n">
+        <v>10</v>
+      </c>
+      <c r="V6" t="n">
+        <v>60</v>
+      </c>
+      <c r="W6" t="n">
+        <v>50</v>
+      </c>
+      <c r="X6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z6" t="inlineStr"/>
+      <c r="AA6" t="inlineStr"/>
+      <c r="AB6" t="inlineStr"/>
+      <c r="AC6" t="inlineStr"/>
+      <c r="AD6" t="n">
+        <v>146.1190349864237</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>0.8547486033519553</v>
+      </c>
+      <c r="AG6" t="inlineStr"/>
+      <c r="AH6" t="n">
+        <v>2</v>
+      </c>
+      <c r="AI6" t="n">
+        <v>32</v>
+      </c>
+      <c r="AJ6" t="n">
+        <v>146.1190349864237</v>
+      </c>
+      <c r="AK6" t="n">
+        <v>2203.2</v>
+      </c>
+      <c r="AL6" t="n">
+        <v>2093.04</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="n">
+        <v>45981</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Build</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Cycling</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Indoor</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>4</v>
+      </c>
+      <c r="F7" t="n">
+        <v>65</v>
+      </c>
+      <c r="G7" t="n">
+        <v>18</v>
+      </c>
+      <c r="H7" t="n">
+        <v>98</v>
+      </c>
+      <c r="I7" t="n">
+        <v>256</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Zone 2</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Mix</t>
+        </is>
+      </c>
+      <c r="L7" t="n">
+        <v>7</v>
+      </c>
+      <c r="M7" t="n">
+        <v>78</v>
+      </c>
+      <c r="N7" t="n">
+        <v>67</v>
+      </c>
+      <c r="O7" t="n">
+        <v>358</v>
+      </c>
+      <c r="P7" t="n">
+        <v>60</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>4480</v>
+      </c>
+      <c r="R7" t="n">
+        <v>1120</v>
+      </c>
+      <c r="S7" t="n">
+        <v>165</v>
+      </c>
+      <c r="T7" t="n">
+        <v>126</v>
+      </c>
+      <c r="U7" t="n">
+        <v>110</v>
+      </c>
+      <c r="V7" t="n">
+        <v>120</v>
+      </c>
+      <c r="W7" t="n">
+        <v>10</v>
+      </c>
+      <c r="X7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z7" t="inlineStr"/>
+      <c r="AA7" t="inlineStr"/>
+      <c r="AB7" t="inlineStr"/>
+      <c r="AC7" t="inlineStr"/>
+      <c r="AD7" t="n">
+        <v>204.537935769795</v>
+      </c>
+      <c r="AE7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF7" t="n">
+        <v>0.7150837988826816</v>
+      </c>
+      <c r="AG7" t="inlineStr"/>
+      <c r="AH7" t="n">
+        <v>4</v>
+      </c>
+      <c r="AI7" t="n">
+        <v>65</v>
+      </c>
+      <c r="AJ7" t="n">
+        <v>204.537935769795</v>
+      </c>
+      <c r="AK7" t="n">
+        <v>3686.4</v>
+      </c>
+      <c r="AL7" t="n">
+        <v>3502.08</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="n">
+        <v>45982</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Build</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Cycling</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Indoor</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>2</v>
+      </c>
+      <c r="F8" t="n">
+        <v>33</v>
+      </c>
+      <c r="G8" t="n">
+        <v>20.1</v>
+      </c>
+      <c r="H8" t="n">
+        <v>77</v>
+      </c>
+      <c r="I8" t="n">
+        <v>268</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Zone 2</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Mix</t>
+        </is>
+      </c>
+      <c r="L8" t="n">
+        <v>8</v>
+      </c>
+      <c r="M8" t="n">
+        <v>89</v>
+      </c>
+      <c r="N8" t="n">
+        <v>77</v>
+      </c>
+      <c r="O8" t="n">
+        <v>358</v>
+      </c>
+      <c r="P8" t="n">
+        <v>60</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>2240</v>
+      </c>
+      <c r="R8" t="n">
+        <v>1120</v>
+      </c>
+      <c r="S8" t="n">
+        <v>145</v>
+      </c>
+      <c r="T8" t="n">
+        <v>122</v>
+      </c>
+      <c r="U8" t="n">
+        <v>60</v>
+      </c>
+      <c r="V8" t="n">
+        <v>60</v>
+      </c>
+      <c r="W8" t="n">
+        <v>0</v>
+      </c>
+      <c r="X8" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z8" t="inlineStr"/>
+      <c r="AA8" t="inlineStr"/>
+      <c r="AB8" t="inlineStr"/>
+      <c r="AC8" t="inlineStr"/>
+      <c r="AD8" t="n">
+        <v>112.0813957117443</v>
+      </c>
+      <c r="AE8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF8" t="n">
+        <v>0.7486033519553073</v>
+      </c>
+      <c r="AG8" t="inlineStr"/>
+      <c r="AH8" t="n">
+        <v>2</v>
+      </c>
+      <c r="AI8" t="n">
+        <v>33</v>
+      </c>
+      <c r="AJ8" t="n">
+        <v>112.0813957117443</v>
+      </c>
+      <c r="AK8" t="n">
+        <v>1929.6</v>
+      </c>
+      <c r="AL8" t="n">
+        <v>1833.12</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="n">
+        <v>45983</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Build</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Cycling</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Outdoor</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>3</v>
+      </c>
+      <c r="F9" t="n">
+        <v>45</v>
+      </c>
+      <c r="G9" t="n">
+        <v>14.5</v>
+      </c>
+      <c r="H9" t="n">
+        <v>89</v>
+      </c>
+      <c r="I9" t="n">
+        <v>245</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Zone 2</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>Mix</t>
+        </is>
+      </c>
+      <c r="L9" t="n">
+        <v>12</v>
+      </c>
+      <c r="M9" t="n">
+        <v>88</v>
+      </c>
+      <c r="N9" t="n">
+        <v>98</v>
+      </c>
+      <c r="O9" t="n">
+        <v>358</v>
+      </c>
+      <c r="P9" t="n">
+        <v>60</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>2240</v>
+      </c>
+      <c r="R9" t="n">
+        <v>746.6666666666666</v>
+      </c>
+      <c r="S9" t="n">
+        <v>136</v>
+      </c>
+      <c r="T9" t="n">
+        <v>115</v>
+      </c>
+      <c r="U9" t="n">
+        <v>50</v>
+      </c>
+      <c r="V9" t="n">
+        <v>130</v>
+      </c>
+      <c r="W9" t="n">
+        <v>0</v>
+      </c>
+      <c r="X9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z9" t="inlineStr"/>
+      <c r="AA9" t="inlineStr"/>
+      <c r="AB9" t="inlineStr"/>
+      <c r="AC9" t="inlineStr"/>
+      <c r="AD9" t="n">
+        <v>140.5035735463937</v>
+      </c>
+      <c r="AE9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF9" t="n">
+        <v>0.6843575418994413</v>
+      </c>
+      <c r="AG9" t="inlineStr"/>
+      <c r="AH9" t="n">
+        <v>3</v>
+      </c>
+      <c r="AI9" t="n">
+        <v>45</v>
+      </c>
+      <c r="AJ9" t="n">
+        <v>140.5035735463937</v>
+      </c>
+      <c r="AK9" t="n">
+        <v>2646</v>
+      </c>
+      <c r="AL9" t="n">
+        <v>2513.7</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="n">
+        <v>45984</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Build</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Cycling</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Outdoor</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>2</v>
+      </c>
+      <c r="F10" t="n">
+        <v>34</v>
+      </c>
+      <c r="G10" t="n">
+        <v>19</v>
+      </c>
+      <c r="H10" t="n">
+        <v>77</v>
+      </c>
+      <c r="I10" t="n">
+        <v>289</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Zone 2</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>Mix</t>
+        </is>
+      </c>
+      <c r="L10" t="n">
+        <v>10</v>
+      </c>
+      <c r="M10" t="n">
+        <v>87</v>
+      </c>
+      <c r="N10" t="n">
+        <v>87</v>
+      </c>
+      <c r="O10" t="n">
+        <v>358</v>
+      </c>
+      <c r="P10" t="n">
+        <v>60</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>2240</v>
+      </c>
+      <c r="R10" t="n">
+        <v>1120</v>
+      </c>
+      <c r="S10" t="n">
+        <v>148</v>
+      </c>
+      <c r="T10" t="n">
+        <v>119</v>
+      </c>
+      <c r="U10" t="n">
+        <v>20</v>
+      </c>
+      <c r="V10" t="n">
+        <v>40</v>
+      </c>
+      <c r="W10" t="n">
+        <v>60</v>
+      </c>
+      <c r="X10" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z10" t="inlineStr"/>
+      <c r="AA10" t="inlineStr"/>
+      <c r="AB10" t="inlineStr"/>
+      <c r="AC10" t="inlineStr"/>
+      <c r="AD10" t="n">
+        <v>130.3345713304828</v>
+      </c>
+      <c r="AE10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF10" t="n">
+        <v>0.8072625698324022</v>
+      </c>
+      <c r="AG10" t="inlineStr"/>
+      <c r="AH10" t="n">
+        <v>2</v>
+      </c>
+      <c r="AI10" t="n">
+        <v>34</v>
+      </c>
+      <c r="AJ10" t="n">
+        <v>130.3345713304828</v>
+      </c>
+      <c r="AK10" t="n">
+        <v>2080.8</v>
+      </c>
+      <c r="AL10" t="n">
+        <v>1976.76</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="n">
+        <v>45985</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Build</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Cycling</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Outdoor</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>3</v>
+      </c>
+      <c r="F11" t="n">
+        <v>56</v>
+      </c>
+      <c r="G11" t="n">
+        <v>18</v>
+      </c>
+      <c r="H11" t="n">
+        <v>54</v>
+      </c>
+      <c r="I11" t="n">
+        <v>267</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Zone 2</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>Mix</t>
+        </is>
+      </c>
+      <c r="L11" t="n">
+        <v>7</v>
+      </c>
+      <c r="M11" t="n">
+        <v>67</v>
+      </c>
+      <c r="N11" t="n">
+        <v>75</v>
+      </c>
+      <c r="O11" t="n">
+        <v>358</v>
+      </c>
+      <c r="P11" t="n">
+        <v>60</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>2240</v>
+      </c>
+      <c r="R11" t="n">
+        <v>746.6666666666666</v>
+      </c>
+      <c r="S11" t="n">
+        <v>156</v>
+      </c>
+      <c r="T11" t="n">
+        <v>126</v>
+      </c>
+      <c r="U11" t="n">
+        <v>10</v>
+      </c>
+      <c r="V11" t="n">
+        <v>50</v>
+      </c>
+      <c r="W11" t="n">
+        <v>75</v>
+      </c>
+      <c r="X11" t="n">
+        <v>15</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z11" t="inlineStr"/>
+      <c r="AA11" t="inlineStr"/>
+      <c r="AB11" t="inlineStr"/>
+      <c r="AC11" t="inlineStr"/>
+      <c r="AD11" t="n">
+        <v>166.8697918292188</v>
+      </c>
+      <c r="AE11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF11" t="n">
+        <v>0.7458100558659218</v>
+      </c>
+      <c r="AG11" t="inlineStr"/>
+      <c r="AH11" t="n">
+        <v>3</v>
+      </c>
+      <c r="AI11" t="n">
+        <v>56</v>
+      </c>
+      <c r="AJ11" t="n">
+        <v>166.8697918292188</v>
+      </c>
+      <c r="AK11" t="n">
+        <v>2883.6</v>
+      </c>
+      <c r="AL11" t="n">
+        <v>2739.42</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="n">
+        <v>45986</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Build</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Cycling</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Outdoor</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>3</v>
+      </c>
+      <c r="F12" t="n">
+        <v>62</v>
+      </c>
+      <c r="G12" t="n">
+        <v>20.1</v>
+      </c>
+      <c r="H12" t="n">
+        <v>54</v>
+      </c>
+      <c r="I12" t="n">
+        <v>290</v>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Zone 3</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>Mix</t>
+        </is>
+      </c>
+      <c r="L12" t="n">
+        <v>9</v>
+      </c>
+      <c r="M12" t="n">
+        <v>89</v>
+      </c>
+      <c r="N12" t="n">
+        <v>78</v>
+      </c>
+      <c r="O12" t="n">
+        <v>358</v>
+      </c>
+      <c r="P12" t="n">
+        <v>60</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>2240</v>
+      </c>
+      <c r="R12" t="n">
+        <v>746.6666666666666</v>
+      </c>
+      <c r="S12" t="n">
+        <v>168</v>
+      </c>
+      <c r="T12" t="n">
+        <v>136</v>
+      </c>
+      <c r="U12" t="n">
+        <v>15</v>
+      </c>
+      <c r="V12" t="n">
+        <v>45</v>
+      </c>
+      <c r="W12" t="n">
+        <v>60</v>
+      </c>
+      <c r="X12" t="n">
+        <v>60</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z12" t="inlineStr"/>
+      <c r="AA12" t="inlineStr"/>
+      <c r="AB12" t="inlineStr"/>
+      <c r="AC12" t="inlineStr"/>
+      <c r="AD12" t="n">
+        <v>196.8571517742892</v>
+      </c>
+      <c r="AE12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF12" t="n">
+        <v>0.8100558659217877</v>
+      </c>
+      <c r="AG12" t="inlineStr"/>
+      <c r="AH12" t="n">
+        <v>3</v>
+      </c>
+      <c r="AI12" t="n">
+        <v>62</v>
+      </c>
+      <c r="AJ12" t="n">
+        <v>196.8571517742892</v>
+      </c>
+      <c r="AK12" t="n">
+        <v>3132</v>
+      </c>
+      <c r="AL12" t="n">
+        <v>2975.4</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="n">
+        <v>45987</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Build</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Cycling</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Outdoor</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>3</v>
+      </c>
+      <c r="F13" t="n">
+        <v>54</v>
+      </c>
+      <c r="G13" t="n">
+        <v>19</v>
+      </c>
+      <c r="H13" t="n">
+        <v>56</v>
+      </c>
+      <c r="I13" t="n">
+        <v>276</v>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Zone 2</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>Mix</t>
+        </is>
+      </c>
+      <c r="L13" t="n">
+        <v>8</v>
+      </c>
+      <c r="M13" t="n">
+        <v>78</v>
+      </c>
+      <c r="N13" t="n">
+        <v>87</v>
+      </c>
+      <c r="O13" t="n">
+        <v>358</v>
+      </c>
+      <c r="P13" t="n">
+        <v>60</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>2240</v>
+      </c>
+      <c r="R13" t="n">
+        <v>746.6666666666666</v>
+      </c>
+      <c r="S13" t="n">
+        <v>169</v>
+      </c>
+      <c r="T13" t="n">
+        <v>134</v>
+      </c>
+      <c r="U13" t="n">
+        <v>60</v>
+      </c>
+      <c r="V13" t="n">
+        <v>60</v>
+      </c>
+      <c r="W13" t="n">
+        <v>60</v>
+      </c>
+      <c r="X13" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z13" t="inlineStr"/>
+      <c r="AA13" t="inlineStr"/>
+      <c r="AB13" t="inlineStr"/>
+      <c r="AC13" t="inlineStr"/>
+      <c r="AD13" t="n">
+        <v>178.3090415405262</v>
+      </c>
+      <c r="AE13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF13" t="n">
+        <v>0.770949720670391</v>
+      </c>
+      <c r="AG13" t="inlineStr"/>
+      <c r="AH13" t="n">
+        <v>3</v>
+      </c>
+      <c r="AI13" t="n">
+        <v>54</v>
+      </c>
+      <c r="AJ13" t="n">
+        <v>178.3090415405262</v>
+      </c>
+      <c r="AK13" t="n">
+        <v>2980.8</v>
+      </c>
+      <c r="AL13" t="n">
+        <v>2831.76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>